<commit_message>
New pin definitions, File size 8 MB
</commit_message>
<xml_diff>
--- a/SD_Card/DOC/read write speed.xlsx
+++ b/SD_Card/DOC/read write speed.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aljaz\GitHub\ESP32_Test\SD_Card\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56520818-3085-4053-B598-44BA902FD102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFD4083-B39D-4B22-B01D-F95DC3235A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{3ABEF9AB-19FE-49B4-8780-D1EA5C2E2CA4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="8 MB file size" sheetId="2" r:id="rId1"/>
+    <sheet name="1 MB file size" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>f MHz</t>
   </si>
@@ -70,10 +71,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -100,9 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,7 +212,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$6</c:f>
+              <c:f>'8 MB file size'!$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -236,7 +247,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
+              <c:f>'8 MB file size'!$B$7:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -275,7 +286,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$16</c:f>
+              <c:f>'8 MB file size'!$C$7:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -301,7 +312,7 @@
                   <c:v>890</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>784</c:v>
+                  <c:v>6227</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>784</c:v>
@@ -315,7 +326,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A517-4D2F-AE10-B28B1CAA370A}"/>
+              <c16:uniqueId val="{00000000-1E23-4366-90FE-5F14754A9210}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -324,7 +335,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>'8 MB file size'!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -359,7 +370,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
+              <c:f>'8 MB file size'!$B$7:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -398,7 +409,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$16</c:f>
+              <c:f>'8 MB file size'!$D$7:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -424,7 +435,7 @@
                   <c:v>2557</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2469</c:v>
+                  <c:v>19762</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2477</c:v>
@@ -438,7 +449,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A517-4D2F-AE10-B28B1CAA370A}"/>
+              <c16:uniqueId val="{00000001-1E23-4366-90FE-5F14754A9210}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -741,7 +752,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>'8 MB file size'!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -776,7 +787,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$16</c:f>
+              <c:f>'8 MB file size'!$F$7:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -815,7 +826,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$16</c:f>
+              <c:f>'8 MB file size'!$G$7:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -841,7 +852,7 @@
                   <c:v>1178.1752808988765</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1337.4693877551019</c:v>
+                  <c:v>1346.8058455114822</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1337.4693877551019</c:v>
@@ -855,7 +866,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-26EE-4D85-A198-D7A5A8B4AA05}"/>
+              <c16:uniqueId val="{00000000-8EB3-44F6-B141-3CEF9FDC413F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -864,7 +875,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$6</c:f>
+              <c:f>'8 MB file size'!$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -899,7 +910,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$16</c:f>
+              <c:f>'8 MB file size'!$F$7:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -938,7 +949,1087 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$16</c:f>
+              <c:f>'8 MB file size'!$H$7:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>252.97370325693606</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>299.08043354249855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340.66796621182584</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>363.0803324099723</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>396.43705103969756</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>408.16504476449978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>410.08056315995304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>424.3780993826536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>423.32498990714572</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>405.32508697332815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8EB3-44F6-B141-3CEF9FDC413F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1616730496"/>
+        <c:axId val="1616741536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1616730496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1616741536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1616741536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1616730496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>time</a:t>
+            </a:r>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 MB file size'!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>read ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$B$7:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$C$7:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2488</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1419</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1209</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>782</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A517-4D2F-AE10-B28B1CAA370A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 MB file size'!$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>write ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$B$7:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$D$7:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3506</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3078</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2888</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2569</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2469</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2477</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2587</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A517-4D2F-AE10-B28B1CAA370A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1345706144"/>
+        <c:axId val="1345707104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1345706144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1345707104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1345707104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1345706144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>speed</a:t>
+            </a:r>
+            <a:endParaRPr lang="sl-SI"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 MB file size'!$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Read kB / s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$F$7:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$G$7:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>421.45337620578778</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>567.10438074634942</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>738.95419309372801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>867.30851943755169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1052.7871485943774</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1176.8529741863076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1178.1752808988765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1337.4693877551019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1337.4693877551019</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1340.8900255754477</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26EE-4D85-A198-D7A5A8B4AA05}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 MB file size'!$H$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Write kB / s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$F$7:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1 MB file size'!$H$7:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1280,6 +2371,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2312,7 +3483,1120 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>621506</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D08EC0-F585-4306-9E0A-8D55636FF497}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>288131</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>326231</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67D01BE1-25CE-43AE-8C67-9351BD3DC6D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2685,10 +4969,317 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8A8434-0F64-4516-AD05-7433AE4F5B02}">
+  <dimension ref="B2:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>8386560</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="str">
+        <f>B6</f>
+        <v>f MHz</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2488</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4145</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F16" si="0">B7</f>
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <f>$F$3/C7</f>
+        <v>421.45337620578778</v>
+      </c>
+      <c r="H7" s="2">
+        <f>$F$3/D7</f>
+        <v>252.97370325693606</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1849</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3506</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G8" s="2">
+        <f>$F$3/C8</f>
+        <v>567.10438074634942</v>
+      </c>
+      <c r="H8" s="2">
+        <f>$F$3/D8</f>
+        <v>299.08043354249855</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1419</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3078</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <f>$F$3/C9</f>
+        <v>738.95419309372801</v>
+      </c>
+      <c r="H9" s="2">
+        <f>$F$3/D9</f>
+        <v>340.66796621182584</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1209</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2888</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G10" s="2">
+        <f>$F$3/C10</f>
+        <v>867.30851943755169</v>
+      </c>
+      <c r="H10" s="2">
+        <f>$F$3/D10</f>
+        <v>363.0803324099723</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3">
+        <v>996</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2645</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G11" s="2">
+        <f>$F$3/C11</f>
+        <v>1052.7871485943774</v>
+      </c>
+      <c r="H11" s="2">
+        <f>$F$3/D11</f>
+        <v>396.43705103969756</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>891</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2569</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G12" s="2">
+        <f>$F$3/C12</f>
+        <v>1176.8529741863076</v>
+      </c>
+      <c r="H12" s="2">
+        <f>$F$3/D12</f>
+        <v>408.16504476449978</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3">
+        <v>890</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2557</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G13" s="2">
+        <f>$F$3/C13</f>
+        <v>1178.1752808988765</v>
+      </c>
+      <c r="H13" s="2">
+        <f>$F$3/D13</f>
+        <v>410.08056315995304</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>6227</v>
+      </c>
+      <c r="D14">
+        <v>19762</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G14" s="1">
+        <f>$F$4/C14</f>
+        <v>1346.8058455114822</v>
+      </c>
+      <c r="H14" s="1">
+        <f>$F$4/D14</f>
+        <v>424.3780993826536</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3">
+        <v>784</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2477</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G15" s="2">
+        <f>$F$3/C15</f>
+        <v>1337.4693877551019</v>
+      </c>
+      <c r="H15" s="2">
+        <f>$F$3/D15</f>
+        <v>423.32498990714572</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>782</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2587</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G16" s="2">
+        <f>$F$3/C16</f>
+        <v>1340.8900255754477</v>
+      </c>
+      <c r="H16" s="2">
+        <f>$F$3/D16</f>
+        <v>405.32508697332815</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44B058C-21A5-4F83-94EF-29B28E24A762}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>